<commit_message>
data bug fix commit 2
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\litfind\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68A975-610E-4017-B974-B034E9DC52CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E495314-4B04-41B8-A69B-47E072A0873F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9407" uniqueCount="4059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9408" uniqueCount="4059">
   <si>
     <t>강경애</t>
   </si>
@@ -14235,8 +14235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A871A3E-29B2-4725-A114-674E3D4FE56E}">
   <dimension ref="A1:J2050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1488" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1499" sqref="B1499"/>
+    <sheetView tabSelected="1" topLeftCell="G2030" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2050" sqref="J2050"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
@@ -46214,7 +46214,9 @@
       </c>
       <c r="H1499" s="8"/>
       <c r="I1499" s="7"/>
-      <c r="J1499" s="8"/>
+      <c r="J1499" s="8" t="s">
+        <v>2285</v>
+      </c>
     </row>
     <row r="1500" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1500" s="3" t="s">

</xml_diff>